<commit_message>
added viz=true to Tutorial file and cleaned up UI + strings
</commit_message>
<xml_diff>
--- a/src/client/assets/documents/script-lab-tutorial.xlsx
+++ b/src/client/assets/documents/script-lab-tutorial.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17524"/>
-  <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\agaves\script lab\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18108"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1200" windowWidth="27150" windowHeight="14970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -283,13 +278,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2333626</xdr:colOff>
+      <xdr:colOff>2971801</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>43007</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>3667126</xdr:colOff>
+      <xdr:colOff>4305301</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>27767</xdr:rowOff>
     </xdr:to>
@@ -307,7 +302,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2333626" y="9301307"/>
+          <a:off x="2971801" y="9301307"/>
           <a:ext cx="1333500" cy="365760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -472,37 +467,7 @@
               <a:ea typeface="Segoe" charset="0"/>
               <a:cs typeface="Segoe" charset="0"/>
             </a:rPr>
-            <a:t> Script lab t</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="Segoe" charset="0"/>
-              <a:cs typeface="Segoe" charset="0"/>
-            </a:rPr>
-            <a:t>o</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" i="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="Segoe" charset="0"/>
-              <a:cs typeface="Segoe" charset="0"/>
-            </a:rPr>
-            <a:t> finish loading it in the pane.</a:t>
+            <a:t> Script Lab and Launch the Code pane.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1200" b="0" i="0">
             <a:solidFill>
@@ -524,15 +489,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>743605</xdr:colOff>
+      <xdr:colOff>200680</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>75356</xdr:rowOff>
+      <xdr:rowOff>65831</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2572405</xdr:colOff>
+      <xdr:colOff>2029480</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>75359</xdr:rowOff>
+      <xdr:rowOff>65834</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -555,7 +520,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="743605" y="1446956"/>
+          <a:off x="200680" y="1437431"/>
           <a:ext cx="1828800" cy="1828803"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -568,15 +533,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1827440</xdr:colOff>
+      <xdr:colOff>1455965</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>58876</xdr:rowOff>
+      <xdr:rowOff>77926</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2373664</xdr:colOff>
+      <xdr:colOff>2002189</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>25117</xdr:rowOff>
+      <xdr:rowOff>44167</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -599,7 +564,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1827440" y="2802076"/>
+          <a:off x="1455965" y="2821126"/>
           <a:ext cx="546224" cy="423441"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -612,15 +577,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>613796</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>217232</xdr:rowOff>
+      <xdr:colOff>851921</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>7682</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>209551</xdr:colOff>
+      <xdr:colOff>447676</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -635,8 +600,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="613796" y="445832"/>
-          <a:ext cx="2977130" cy="278068"/>
+          <a:off x="851921" y="464882"/>
+          <a:ext cx="4348730" cy="278068"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -694,7 +659,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Create, run and share Office API snippets.</a:t>
+            <a:t>Create, run, and share Office API snippets.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1200">
             <a:solidFill>
@@ -713,15 +678,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>623064</xdr:colOff>
+      <xdr:colOff>861189</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2771775</xdr:colOff>
+      <xdr:colOff>3009900</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
+      <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -736,7 +701,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="623064" y="133350"/>
+          <a:off x="861189" y="152400"/>
           <a:ext cx="2148711" cy="400051"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -805,15 +770,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>196283</xdr:colOff>
+      <xdr:colOff>434408</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1472</xdr:rowOff>
+      <xdr:rowOff>20522</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>603366</xdr:colOff>
+      <xdr:colOff>841491</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>184091</xdr:rowOff>
+      <xdr:rowOff>203141</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -836,7 +801,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="196283" y="230072"/>
+          <a:off x="434408" y="249122"/>
           <a:ext cx="407083" cy="411219"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1066,7 +1031,7 @@
               <a:ea typeface="Segoe" charset="0"/>
               <a:cs typeface="Segoe" charset="0"/>
             </a:rPr>
-            <a:t> fit, enlarge to Code pane</a:t>
+            <a:t> fit, enlarge the Code pane</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" i="0" baseline="0">
@@ -1103,15 +1068,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>747711</xdr:colOff>
+      <xdr:colOff>214311</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2576510</xdr:colOff>
+      <xdr:colOff>2043110</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>95253</xdr:rowOff>
+      <xdr:rowOff>47628</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1134,7 +1099,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="747711" y="3752850"/>
+          <a:off x="214311" y="3705225"/>
           <a:ext cx="1828799" cy="1828803"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1147,15 +1112,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>161923</xdr:colOff>
+      <xdr:colOff>390523</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>3139053</xdr:colOff>
+      <xdr:colOff>3952875</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1170,8 +1135,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="161923" y="819149"/>
-          <a:ext cx="2977130" cy="466725"/>
+          <a:off x="390523" y="838199"/>
+          <a:ext cx="3562352" cy="466725"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1229,7 +1194,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>This tutorial will introduce you to a basic Script Lab coding workflow. Let's set up first,</a:t>
+            <a:t>This tutorial will introduce you to a basic Script Lab coding workflow. Let's set up first:</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1200">
             <a:solidFill>
@@ -1325,6 +1290,94 @@
         <a:xfrm>
           <a:off x="1266825" y="8229600"/>
           <a:ext cx="546224" cy="414247"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2305050</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4241426</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AB1CD45-ECCA-41FD-B799-B534045F823C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2305050" y="1438275"/>
+          <a:ext cx="1936376" cy="1885950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2945342</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>135739</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3491566</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>85438</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33234A3A-DA69-4D78-AD1F-343D85925EAB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2945342" y="2878939"/>
+          <a:ext cx="546224" cy="406899"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1940,7 +1993,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Open the Run pane from the Script Lab tab to code and run your snippet side by side.</a:t>
+            <a:t>Open the Run pane from the Script Lab tab to code and run side-by-side.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2178,7 +2231,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Select the first cell to color it</a:t>
+            <a:t>Select the cell to color it</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2591,7 +2644,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>In the run pane, click the Run Code button to color the cell with  yellow.</a:t>
+            <a:t>In the run pane, click the Run Code button to color the cell yellow.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1200">
             <a:solidFill>
@@ -4492,7 +4545,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Check out other samples in the  </a:t>
+            <a:t>Check out other samples in the </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1" i="0" baseline="0">
@@ -4522,7 +4575,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> section to play and learn about other Office API's.</a:t>
+            <a:t> section to learn about the rest of the Office JavaScript API.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1200">
             <a:solidFill>
@@ -4580,7 +4633,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>You can share your code snippets as gists directly from the Script Lab add-in and to the developer community by signing in to your GitHub account.</a:t>
+            <a:t>You can share your code snippets as gists directly from Script Lab by signing in to your GitHub account.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1200">
             <a:solidFill>
@@ -5137,7 +5190,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="Segoe UI Semibold" panose="020B0702040204020203" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Office API's</a:t>
+            <a:t>Office JavaScript API</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -5155,7 +5208,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>Learn about Office API's and </a:t>
+            <a:t>Learn about the API and </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -5173,7 +5226,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>the functionalities they offer.</a:t>
+            <a:t>the functionality it offers</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1200">
             <a:solidFill>
@@ -5515,7 +5568,7 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="0">
+            <a:rPr lang="en-US" sz="1200" u="none" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -5527,22 +5580,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" u="sng" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>UX</a:t>
+            <a:t>UX </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200" baseline="0">
@@ -5557,7 +5595,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t> documentation and </a:t>
+            <a:t>documentation and </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -5575,7 +5613,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>design recommendations.</a:t>
+            <a:t>design recommendations</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1200">
             <a:solidFill>
@@ -23670,69 +23708,15 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="397" row="3">
+  <wetp:taskpane dockstate="right" visibility="1" width="350" row="3">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-  </wetp:taskpane>
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="2">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-  </wetp:taskpane>
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="3">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-  </wetp:taskpane>
-  <wetp:taskpane dockstate="right" visibility="0" width="826" row="10">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-  </wetp:taskpane>
-  <wetp:taskpane dockstate="right" visibility="0" width="575" row="21">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{87AB2A74-FAEC-4D84-8E38-656E7C5218A2}">
-  <we:reference id="295fd99e-ae9d-4140-8f93-f1916e904c52" version="1.0.0.2" store="\\officefile\public\danielmg\manifests\" storeType="Filesystem"/>
-  <we:alternateReferences/>
-  <we:properties/>
-  <we:bindings/>
-  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</we:webextension>
-</file>
-
-<file path=xl/webextensions/webextension2.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{874C79D0-137C-45BD-A762-79885541E317}">
-  <we:reference id="wa104126656" version="1.0.0.0" store="en-US" storeType="OMEX"/>
-  <we:alternateReferences>
-    <we:reference id="wa104126656" version="1.0.0.0" store="wa104126656" storeType="OMEX"/>
-  </we:alternateReferences>
-  <we:properties/>
-  <we:bindings/>
-  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</we:webextension>
-</file>
-
-<file path=xl/webextensions/webextension3.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{BDC676D9-4F3D-4279-BE8B-EE21FC0C645F}">
-  <we:reference id="629ed84c-2c4a-4e4b-bc87-353bcf7a34d5" version="1.0.0.3" store="\\JDMGSURFACE\danimanifests" storeType="Filesystem"/>
-  <we:alternateReferences/>
-  <we:properties/>
-  <we:bindings/>
-  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</we:webextension>
-</file>
-
-<file path=xl/webextensions/webextension4.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{DA8D7A25-7EB9-4D65-9CD1-D67E58581A0D}">
-  <we:reference id="98630478-cf6b-4761-b560-cfb857741f2b" version="1.0.0.4" store="\\DANIELPC\Users\v-jmoasr\Desktop\manifests" storeType="Filesystem"/>
-  <we:alternateReferences/>
-  <we:properties/>
-  <we:bindings/>
-  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</we:webextension>
-</file>
-
-<file path=xl/webextensions/webextension5.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{DF567FB5-2E62-4E4B-AFE0-208B260E6F4E}">
-  <we:reference id="b6812bee-73bd-48a8-b70d-755bd1a510ef" version="1.0.0.4" store="\\DANIELPC\Users\v-jmoasr\Desktop\manifests" storeType="Filesystem"/>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{635BF0CD-42CC-4174-B8D2-6D375C9A759E}">
+  <we:reference id="wa104380862" version="1.1.0.0" store="en-US" storeType="OMEX"/>
   <we:alternateReferences/>
   <we:properties/>
   <we:bindings/>
@@ -23746,12 +23730,12 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D10" sqref="D10"/>
+      <selection pane="topRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57" style="4" customWidth="1"/>
+    <col min="1" max="1" width="67" style="4" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" customWidth="1"/>
     <col min="3" max="24" width="7.7109375" customWidth="1"/>
     <col min="25" max="25" width="9.7109375" customWidth="1"/>
@@ -23798,7 +23782,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G9" sqref="G9"/>
+      <selection pane="topRight" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23846,9 +23830,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H3" sqref="H3"/>
+      <selection pane="topRight" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23898,7 +23882,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H4" sqref="H4"/>
+      <selection pane="topRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23937,7 +23921,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B18" sqref="B18"/>
+      <selection pane="topRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24170,286 +24154,4 @@
   <pageSetup orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="4f31bb54-1ffc-4ceb-8b46-9126da6f81ff">
-      <UserInfo>
-        <DisplayName>Jakob Nielsen (OFFICE)</DisplayName>
-        <AccountId>127</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Michael Saunders (OFFICE)</DisplayName>
-        <AccountId>727</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Michael Zlatkovsky</DisplayName>
-        <AccountId>720</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Bhargav Krishna</DisplayName>
-        <AccountId>199</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010089AEB9B9D5EB5E40AD89B88E1B459A06" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5c4e7d5d038fb12afbf6bf85d1b9ac15">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4f31bb54-1ffc-4ceb-8b46-9126da6f81ff" xmlns:ns3="0cad17d5-cabb-42bc-8466-cf805e49c806" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="65a655ba931daddcb23821d3b6a398a8" ns1:_="" ns2:_="" ns3:_="">
-    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
-    <xsd:import namespace="4f31bb54-1ffc-4ceb-8b46-9126da6f81ff"/>
-    <xsd:import namespace="0cad17d5-cabb-42bc-8466-cf805e49c806"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns2:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns2:LastSharedByUser" minOccurs="0"/>
-                <xsd:element ref="ns2:LastSharedByTime" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
-                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="14" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:description="" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="15" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:description="" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="4f31bb54-1ffc-4ceb-8b46-9126da6f81ff" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:description="" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:description="" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LastSharedByUser" ma:index="10" nillable="true" ma:displayName="Last Shared By User" ma:description="" ma:internalName="LastSharedByUser" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="LastSharedByTime" ma:index="11" nillable="true" ma:displayName="Last Shared By Time" ma:description="" ma:internalName="LastSharedByTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:DateTime"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="0cad17d5-cabb-42bc-8466-cf805e49c806" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="12" nillable="true" ma:displayName="MediaServiceMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="13" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D7075C9-3206-408E-AAD9-E1DB263C49C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="4f31bb54-1ffc-4ceb-8b46-9126da6f81ff"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="0cad17d5-cabb-42bc-8466-cf805e49c806"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92268FE7-B501-4581-BB47-BE80D3A9E9AD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="4f31bb54-1ffc-4ceb-8b46-9126da6f81ff"/>
-    <ds:schemaRef ds:uri="0cad17d5-cabb-42bc-8466-cf805e49c806"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D750D0D-4639-4B11-A503-F40820F7683F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
tutorial with the Enable Editing instruction added
</commit_message>
<xml_diff>
--- a/src/client/assets/documents/script-lab-tutorial.xlsx
+++ b/src/client/assets/documents/script-lab-tutorial.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18108"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="27150" windowHeight="14970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20475" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" r:id="rId1"/>
@@ -386,15 +386,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>321300</xdr:colOff>
+      <xdr:colOff>368925</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>103050</xdr:rowOff>
+      <xdr:rowOff>45900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -409,8 +409,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="321300" y="3303450"/>
-          <a:ext cx="3079125" cy="306525"/>
+          <a:off x="368925" y="3246300"/>
+          <a:ext cx="4164975" cy="306525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -452,7 +452,7 @@
               <a:ea typeface="Segoe" charset="0"/>
               <a:cs typeface="Segoe" charset="0"/>
             </a:rPr>
-            <a:t>Trust</a:t>
+            <a:t>Enable editing and trust</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" i="0" baseline="0">
@@ -467,7 +467,7 @@
               <a:ea typeface="Segoe" charset="0"/>
               <a:cs typeface="Segoe" charset="0"/>
             </a:rPr>
-            <a:t> Script Lab and Launch the Code pane.</a:t>
+            <a:t> Script Lab.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1200" b="0" i="0">
             <a:solidFill>
@@ -489,15 +489,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>200680</xdr:colOff>
+      <xdr:colOff>2258079</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>65831</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2029480</xdr:colOff>
+      <xdr:colOff>4171760</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>65834</xdr:rowOff>
+      <xdr:rowOff>84885</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -520,8 +520,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="200680" y="1437431"/>
-          <a:ext cx="1828800" cy="1828803"/>
+          <a:off x="2258079" y="1371601"/>
+          <a:ext cx="1913681" cy="1913684"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -533,15 +533,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1455965</xdr:colOff>
+      <xdr:colOff>3646715</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>77926</xdr:rowOff>
+      <xdr:rowOff>68401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2002189</xdr:colOff>
+      <xdr:colOff>4192939</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>44167</xdr:rowOff>
+      <xdr:rowOff>34642</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -564,7 +564,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1455965" y="2821126"/>
+          <a:off x="3646715" y="2811601"/>
           <a:ext cx="546224" cy="423441"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -659,7 +659,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Create, run, and share Office API snippets.</a:t>
+            <a:t>Create, run, and share Office JavaScript API snippets</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1200">
             <a:solidFill>
@@ -936,14 +936,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>363141</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>115254</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>10479</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>102392</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>91481</xdr:rowOff>
+      <xdr:rowOff>215306</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -958,8 +958,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="363141" y="5601654"/>
-          <a:ext cx="3120626" cy="662027"/>
+          <a:off x="363141" y="5725479"/>
+          <a:ext cx="4206476" cy="662027"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1001,37 +1001,7 @@
               <a:ea typeface="Segoe" charset="0"/>
               <a:cs typeface="Segoe" charset="0"/>
             </a:rPr>
-            <a:t>For a</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" i="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="Segoe" charset="0"/>
-              <a:cs typeface="Segoe" charset="0"/>
-            </a:rPr>
-            <a:t> better</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="Segoe" charset="0"/>
-              <a:cs typeface="Segoe" charset="0"/>
-            </a:rPr>
-            <a:t> fit, enlarge the Code pane</a:t>
+            <a:t>Launch the Code pane and enlarge it for a better fit</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="0" i="0" baseline="0">
@@ -1068,15 +1038,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>214311</xdr:colOff>
+      <xdr:colOff>2328861</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>200026</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2043110</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>47628</xdr:rowOff>
+      <xdr:colOff>4205285</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>19054</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1099,8 +1069,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="214311" y="3705225"/>
-          <a:ext cx="1828799" cy="1828803"/>
+          <a:off x="2328861" y="3857626"/>
+          <a:ext cx="1876424" cy="1876428"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1301,15 +1271,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2305050</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>4241426</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>2155451</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1332,7 +1302,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2305050" y="1438275"/>
+          <a:off x="219075" y="3848100"/>
           <a:ext cx="1936376" cy="1885950"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1345,15 +1315,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2945342</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>135739</xdr:rowOff>
+      <xdr:colOff>802217</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>30964</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>3491566</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>85438</xdr:rowOff>
+      <xdr:colOff>1348441</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>209263</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1376,8 +1346,95 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2945342" y="2878939"/>
+          <a:off x="802217" y="5288764"/>
           <a:ext cx="546224" cy="406899"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>209551</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9106</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2124075</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82FF2FA8-D911-413D-B484-2E97D8336619}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:srcRect l="3662" t="2654" r="2947"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="209551" y="1380706"/>
+          <a:ext cx="1914524" cy="1886369"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1533525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2079749</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>156741</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57C6C2C5-E917-4040-8B7D-FF505B7FDB84}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1533525" y="2019300"/>
+          <a:ext cx="546224" cy="423441"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -23730,7 +23787,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D12" sqref="D12"/>
+      <selection pane="topRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated tutorial to have setting for taskpane auto-open
</commit_message>
<xml_diff>
--- a/src/client/assets/documents/script-lab-tutorial.xlsx
+++ b/src/client/assets/documents/script-lab-tutorial.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18110"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20475" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -23765,7 +23765,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="1" width="350" row="3">
+  <wetp:taskpane dockstate="right" visibility="1" width="350" row="4">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -23775,7 +23775,9 @@
 <we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{635BF0CD-42CC-4174-B8D2-6D375C9A759E}">
   <we:reference id="wa104380862" version="1.1.0.0" store="en-US" storeType="OMEX"/>
   <we:alternateReferences/>
-  <we:properties/>
+  <we:properties>
+    <we:property name="Office.AutoShowTaskpaneWithDocument" value="true"/>
+  </we:properties>
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </we:webextension>

</xml_diff>